<commit_message>
made all tests independent of each other
</commit_message>
<xml_diff>
--- a/data/unitTests/excelTest/Feriekasse.xlsx
+++ b/data/unitTests/excelTest/Feriekasse.xlsx
@@ -26,13 +26,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <color rgb="00ff0000"/>
-    </font>
-    <font>
       <color rgb="0000ff00"/>
     </font>
     <font>
-      <color rgb="000000ff"/>
+      <color rgb="00000000"/>
+    </font>
+    <font>
+      <color rgb="00ff0000"/>
     </font>
   </fonts>
   <fills count="2">
@@ -466,7 +466,7 @@
         </is>
       </c>
       <c r="B2">
-        <f>0</f>
+        <f>0+20</f>
         <v/>
       </c>
       <c r="C2" s="1" t="inlineStr">
@@ -475,7 +475,7 @@
         </is>
       </c>
       <c r="D2">
-        <f>0</f>
+        <f>0+10</f>
         <v/>
       </c>
       <c r="E2" s="1" t="inlineStr">
@@ -491,7 +491,7 @@
         </is>
       </c>
       <c r="B3">
-        <f>0</f>
+        <f>0+30</f>
         <v/>
       </c>
       <c r="C3" s="2" t="inlineStr">
@@ -500,7 +500,7 @@
         </is>
       </c>
       <c r="D3">
-        <f>0</f>
+        <f>0+40</f>
         <v/>
       </c>
       <c r="E3" s="2" t="inlineStr">

</xml_diff>

<commit_message>
fixed a bug where it would just skip random matches (fx all relagation matches (or those that the site thought was relegation matches) in superligaen)
fixed by getting the table of matches another way
</commit_message>
<xml_diff>
--- a/data/unitTests/excelTest/Feriekasse.xlsx
+++ b/data/unitTests/excelTest/Feriekasse.xlsx
@@ -26,13 +26,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <color rgb="0000ff00"/>
+      <color rgb="00ff00ff"/>
     </font>
     <font>
       <color rgb="00000000"/>
     </font>
     <font>
-      <color rgb="00ff0000"/>
+      <color rgb="0000ff00"/>
     </font>
   </fonts>
   <fills count="2">

</xml_diff>

<commit_message>
added test for util
</commit_message>
<xml_diff>
--- a/data/unitTests/excelTest/Feriekasse.xlsx
+++ b/data/unitTests/excelTest/Feriekasse.xlsx
@@ -26,13 +26,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <color rgb="00ff00ff"/>
+      <color rgb="00ff9933"/>
+    </font>
+    <font>
+      <color rgb="000000ff"/>
     </font>
     <font>
       <color rgb="00000000"/>
-    </font>
-    <font>
-      <color rgb="0000ff00"/>
     </font>
   </fonts>
   <fills count="2">

</xml_diff>